<commit_message>
Update readme and BD
</commit_message>
<xml_diff>
--- a/BD_esmoltificación.xlsx
+++ b/BD_esmoltificación.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paula\Dropbox\PAULA_VALENZUELA\Proyecto-Inmunidad-y-estres\Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3a699629cef954bb/Documentos/GitHub/TareaDBD845/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104A5CA8-35CC-4A59-BBBE-D776362F7906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{B2FFF0ED-DB29-457B-AC48-D7E3AA9B3ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{BD30F603-F07B-482E-AF52-FC895A27AF89}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{BD30F603-F07B-482E-AF52-FC895A27AF89}"/>
   </bookViews>
   <sheets>
     <sheet name="pheno_esmoltificacion" sheetId="1" r:id="rId1"/>
@@ -10132,7 +10132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F73D805-912D-4988-9379-CE00239D1222}">
   <dimension ref="A1:H601"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -25779,7 +25779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB3379FD-2CF5-4A4D-BD6B-81B0D263BEF3}">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A104" workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -28583,8 +28583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B044BD59-25B6-4E2A-9E7A-EABF615CD89E}">
   <dimension ref="A1:T121"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>